<commit_message>
change our template for mass book upload and controller to read it
</commit_message>
<xml_diff>
--- a/public/books_template.xlsx
+++ b/public/books_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="28755" windowHeight="12855"/>
+    <workbookView xWindow="0" yWindow="3885" windowWidth="28755" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
@@ -416,8 +416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -425,13 +425,13 @@
     <col min="2" max="2" width="27.85546875" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" customWidth="1"/>
-    <col min="10" max="10" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="5" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1">
@@ -442,31 +442,31 @@
         <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>